<commit_message>
Change System_init. Model Updated
</commit_message>
<xml_diff>
--- a/Signal_Response_building.xlsx
+++ b/Signal_Response_building.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frederic.amblard\Desktop\Thèse\Models\Sim4Blocks_Naters\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="11">
   <si>
     <t>T_return</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Dt = 15 min</t>
+  </si>
+  <si>
+    <t>Step</t>
   </si>
 </sst>
 </file>
@@ -169,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -180,6 +183,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,20 +466,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G32"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A2:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -493,7 +503,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>0</v>
+      </c>
       <c r="B4" s="4">
         <v>0</v>
       </c>
@@ -513,7 +526,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>1</v>
+      </c>
       <c r="B5" s="4">
         <v>0</v>
       </c>
@@ -533,7 +549,10 @@
         <v>19.999935127721798</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>2</v>
+      </c>
       <c r="B6" s="4">
         <v>0</v>
       </c>
@@ -553,7 +572,10 @@
         <v>19.9998702100823</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>3</v>
+      </c>
       <c r="B7" s="4">
         <v>0</v>
       </c>
@@ -573,7 +595,10 @@
         <v>19.9998053446947</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>4</v>
+      </c>
       <c r="B8" s="7">
         <v>0</v>
       </c>
@@ -593,12 +618,15 @@
         <v>19.999740643787099</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
@@ -618,7 +646,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>0</v>
+      </c>
       <c r="B12" s="4">
         <v>0</v>
       </c>
@@ -638,7 +669,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>1</v>
+      </c>
       <c r="B13" s="4">
         <v>0</v>
       </c>
@@ -658,7 +692,10 @@
         <v>19.996008116976</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>2</v>
+      </c>
       <c r="B14" s="4">
         <v>0</v>
       </c>
@@ -678,7 +715,10 @@
         <v>19.994119015159999</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>3</v>
+      </c>
       <c r="B15" s="4">
         <v>0</v>
       </c>
@@ -698,7 +738,10 @@
         <v>19.998287280868599</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>4</v>
+      </c>
       <c r="B16" s="7">
         <v>0</v>
       </c>
@@ -718,12 +761,15 @@
         <v>20.006702386738102</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>5</v>
       </c>
@@ -743,7 +789,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>0</v>
+      </c>
       <c r="B20" s="4">
         <v>0</v>
       </c>
@@ -763,7 +812,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>1</v>
+      </c>
       <c r="B21" s="4">
         <v>0</v>
       </c>
@@ -774,16 +826,19 @@
         <v>60</v>
       </c>
       <c r="E21" s="5">
-        <v>24.9249120789359</v>
+        <v>24.852767080646</v>
       </c>
       <c r="F21" s="5">
-        <v>21.937274136232201</v>
+        <v>21.856203916320499</v>
       </c>
       <c r="G21" s="6">
-        <v>19.996008116976</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+        <v>19.979146932101699</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>2</v>
+      </c>
       <c r="B22" s="4">
         <v>0</v>
       </c>
@@ -794,16 +849,19 @@
         <v>60</v>
       </c>
       <c r="E22" s="5">
-        <v>34.9828713319705</v>
+        <v>39.0935135148586</v>
       </c>
       <c r="F22" s="5">
-        <v>23.585912186760901</v>
+        <v>27.097694618126699</v>
       </c>
       <c r="G22" s="6">
-        <v>19.994119015159999</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+        <v>20.012470095649402</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>3</v>
+      </c>
       <c r="B23" s="4">
         <v>0</v>
       </c>
@@ -814,16 +872,19 @@
         <v>60</v>
       </c>
       <c r="E23" s="5">
-        <v>37.347045703023802</v>
+        <v>39.425250148468997</v>
       </c>
       <c r="F23" s="5">
-        <v>25.276530112265799</v>
+        <v>27.477551068029499</v>
       </c>
       <c r="G23" s="6">
-        <v>19.998287280868599</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>20.078523817849501</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
+        <v>4</v>
+      </c>
       <c r="B24" s="7">
         <v>0</v>
       </c>
@@ -834,21 +895,24 @@
         <v>60</v>
       </c>
       <c r="E24" s="8">
-        <v>38.329492097350297</v>
+        <v>39.473399561969302</v>
       </c>
       <c r="F24" s="8">
-        <v>26.268380527412599</v>
+        <v>27.547121204466801</v>
       </c>
       <c r="G24" s="9">
-        <v>20.006702386738102</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>20.145770205286599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
@@ -868,7 +932,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>0</v>
+      </c>
       <c r="B28" s="4">
         <v>0</v>
       </c>
@@ -888,7 +955,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>1</v>
+      </c>
       <c r="B29" s="4">
         <v>0</v>
       </c>
@@ -899,16 +969,19 @@
         <v>60</v>
       </c>
       <c r="E29" s="5">
-        <v>24.9249120789359</v>
+        <v>24.825118284210198</v>
       </c>
       <c r="F29" s="5">
-        <v>21.937274136232201</v>
+        <v>21.815252902806201</v>
       </c>
       <c r="G29" s="6">
-        <v>19.996008116976</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+        <v>19.9365266922808</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>2</v>
+      </c>
       <c r="B30" s="4">
         <v>0</v>
       </c>
@@ -919,16 +992,19 @@
         <v>60</v>
       </c>
       <c r="E30" s="5">
-        <v>34.9828713319705</v>
+        <v>39.451806481268498</v>
       </c>
       <c r="F30" s="5">
-        <v>23.585912186760901</v>
+        <v>27.512998054929302</v>
       </c>
       <c r="G30" s="6">
-        <v>19.994119015159999</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+        <v>20.103925531273799</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>3</v>
+      </c>
       <c r="B31" s="4">
         <v>0</v>
       </c>
@@ -939,16 +1015,19 @@
         <v>60</v>
       </c>
       <c r="E31" s="5">
-        <v>37.347045703023802</v>
+        <v>39.555751585439999</v>
       </c>
       <c r="F31" s="5">
-        <v>25.276530112265799</v>
+        <v>27.676952978339699</v>
       </c>
       <c r="G31" s="6">
-        <v>19.998287280868599</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>20.304128387374099</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10">
+        <v>4</v>
+      </c>
       <c r="B32" s="7">
         <v>0</v>
       </c>
@@ -959,13 +1038,13 @@
         <v>60</v>
       </c>
       <c r="E32" s="8">
-        <v>38.329492097350297</v>
+        <v>39.657104806189203</v>
       </c>
       <c r="F32" s="8">
-        <v>26.268380527412599</v>
+        <v>27.837120774334</v>
       </c>
       <c r="G32" s="9">
-        <v>20.006702386738102</v>
+        <v>20.5005428140025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>